<commit_message>
Added "category" and "group" fields to DDS and removed "symbol, sample_value, maximum_value, minimum_value, default_value, input_widget, output_widget" which were unused.
</commit_message>
<xml_diff>
--- a/dds/constants.xlsx
+++ b/dds/constants.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DTOcean_code\dtocean-core\dds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="990" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="129">
   <si>
     <t>Identifier</t>
   </si>
@@ -43,27 +43,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Symbol</t>
-  </si>
-  <si>
-    <t>Sample Value</t>
-  </si>
-  <si>
-    <t>Maximum Value</t>
-  </si>
-  <si>
-    <t>Minimum Value</t>
-  </si>
-  <si>
-    <t>Default Value</t>
-  </si>
-  <si>
-    <t>Input Widget</t>
-  </si>
-  <si>
-    <t>Output Widget</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -428,19 +407,35 @@
   </si>
   <si>
     <t>grout_density</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Auto Only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -464,7 +459,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,14 +468,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF66"/>
-        <bgColor rgb="FF9BBB59"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor rgb="FFFF6600"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -513,18 +502,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -532,18 +520,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -893,25 +880,27 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.85546875"/>
-    <col min="2" max="2" width="29.85546875"/>
-    <col min="3" max="3" width="45.28515625"/>
-    <col min="4" max="4" width="123.85546875"/>
-    <col min="5" max="5" width="19.85546875"/>
-    <col min="6" max="6" width="38.85546875"/>
-    <col min="7" max="1025" width="19.85546875"/>
+    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="1021" width="19.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -925,210 +914,198 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="B3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="B4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="3" t="s">
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
+    </row>
+    <row r="14" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="D14" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1148,200 +1125,200 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.140625"/>
-    <col min="2" max="1025" width="19.85546875"/>
+    <col min="1" max="1" width="38.1796875"/>
+    <col min="2" max="1025" width="19.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="B8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>58</v>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1352,165 +1329,168 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.140625"/>
-    <col min="2" max="2" width="24.5703125"/>
-    <col min="3" max="3" width="34.140625"/>
-    <col min="4" max="4" width="32.85546875"/>
-    <col min="5" max="5" width="26.85546875"/>
-    <col min="6" max="7" width="18.7109375"/>
-    <col min="8" max="9" width="19.7109375"/>
-    <col min="10" max="1025" width="8.42578125"/>
+    <col min="1" max="1" width="36.1796875"/>
+    <col min="2" max="2" width="24.54296875"/>
+    <col min="3" max="3" width="34.1796875"/>
+    <col min="4" max="4" width="32.81640625"/>
+    <col min="5" max="5" width="26.81640625"/>
+    <col min="6" max="7" width="18.7265625"/>
+    <col min="8" max="9" width="19.7265625"/>
+    <col min="10" max="1025" width="8.453125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="F4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="G4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="H4" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="I4" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
         <v>76</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1530,75 +1510,75 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="32"/>
-    <col min="2" max="1025" width="19.85546875"/>
+    <col min="2" max="1025" width="19.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1614,226 +1594,226 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.140625"/>
-    <col min="2" max="2" width="32.7109375"/>
-    <col min="3" max="3" width="25.42578125"/>
-    <col min="4" max="4" width="39.28515625"/>
-    <col min="5" max="5" width="37.7109375"/>
-    <col min="6" max="8" width="21.42578125"/>
-    <col min="9" max="10" width="22.42578125"/>
-    <col min="11" max="1025" width="19.85546875"/>
+    <col min="1" max="1" width="36.1796875"/>
+    <col min="2" max="2" width="32.7265625"/>
+    <col min="3" max="3" width="25.453125"/>
+    <col min="4" max="4" width="39.26953125"/>
+    <col min="5" max="5" width="37.7265625"/>
+    <col min="6" max="8" width="21.453125"/>
+    <col min="9" max="10" width="22.453125"/>
+    <col min="11" max="1025" width="19.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E3" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F3" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="11" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="D4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C5" t="s">
         <v>99</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D5" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="E5" t="s">
         <v>101</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F5" t="s">
         <v>102</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G5" t="s">
         <v>103</v>
       </c>
-      <c r="E4" t="s">
+      <c r="H5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="I5" t="s">
         <v>105</v>
       </c>
-      <c r="C5" t="s">
+      <c r="J5" t="s">
         <v>106</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E5" t="s">
+      <c r="C6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
         <v>108</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D7" t="s">
         <v>109</v>
       </c>
-      <c r="G5" t="s">
-        <v>110</v>
-      </c>
-      <c r="H5" t="s">
-        <v>111</v>
-      </c>
-      <c r="I5" t="s">
-        <v>112</v>
-      </c>
-      <c r="J5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" s="11" t="s">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="11" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
         <v>123</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
         <v>124</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1853,26 +1833,26 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1025" width="19.85546875"/>
+    <col min="1" max="1025" width="19.81640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>120</v>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified database access to require schema to be explicitly given in the DB table definitions.
Updated DDS sheets and configuration to use dtocean_examples DB.
</commit_message>
<xml_diff>
--- a/dds/constants.xlsx
+++ b/dds/constants.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -292,15 +292,9 @@
     <t>Table …</t>
   </si>
   <si>
-    <t>ref_general_parameter</t>
-  </si>
-  <si>
     <t>groutstr</t>
   </si>
   <si>
-    <t>ref_drag_coef_cyl</t>
-  </si>
-  <si>
     <t>reynolds_number</t>
   </si>
   <si>
@@ -313,9 +307,6 @@
     <t>roughness_1e_2</t>
   </si>
   <si>
-    <t>ref_wake_amplification_factor_cyl</t>
-  </si>
-  <si>
     <t>kc_steady_drag_coefficient</t>
   </si>
   <si>
@@ -325,9 +316,6 @@
     <t>amplification_factor_for_rough_cylinders</t>
   </si>
   <si>
-    <t>ref_wind_drag_coef_rect</t>
-  </si>
-  <si>
     <t>width_length</t>
   </si>
   <si>
@@ -352,9 +340,6 @@
     <t>height_breadth_less_20</t>
   </si>
   <si>
-    <t>ref_current_drag_coef_rect</t>
-  </si>
-  <si>
     <t>wavenumber_draft</t>
   </si>
   <si>
@@ -373,24 +358,15 @@
     <t>Value …</t>
   </si>
   <si>
-    <t>ref_drift_coef_float_rect</t>
-  </si>
-  <si>
     <t>thickness_width</t>
   </si>
   <si>
-    <t>ref_rectangular_wave_inertia</t>
-  </si>
-  <si>
     <t>width/length</t>
   </si>
   <si>
     <t>inertia_coefficients</t>
   </si>
   <si>
-    <t>constants</t>
-  </si>
-  <si>
     <t>gravity</t>
   </si>
   <si>
@@ -416,6 +392,30 @@
   </si>
   <si>
     <t>Auto Only</t>
+  </si>
+  <si>
+    <t>reference.ref_general_parameter</t>
+  </si>
+  <si>
+    <t>reference.ref_wake_amplification_factor_cyl</t>
+  </si>
+  <si>
+    <t>reference.ref_drag_coef_cyl</t>
+  </si>
+  <si>
+    <t>reference.ref_wind_drag_coef_rect</t>
+  </si>
+  <si>
+    <t>reference.ref_current_drag_coef_rect</t>
+  </si>
+  <si>
+    <t>reference.ref_drift_coef_float_rect</t>
+  </si>
+  <si>
+    <t>reference.ref_rectangular_wave_inertia</t>
+  </si>
+  <si>
+    <t>reference.constants</t>
   </si>
 </sst>
 </file>
@@ -882,7 +882,7 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
@@ -914,13 +914,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1594,14 +1594,14 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.1796875"/>
-    <col min="2" max="2" width="32.7265625"/>
+    <col min="2" max="2" width="43.54296875" customWidth="1"/>
     <col min="3" max="3" width="25.453125"/>
     <col min="4" max="4" width="39.26953125"/>
     <col min="5" max="5" width="37.7265625"/>
@@ -1633,10 +1633,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
         <v>87</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1644,36 +1644,36 @@
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>91</v>
       </c>
-      <c r="E3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1681,31 +1681,31 @@
         <v>34</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" t="s">
         <v>98</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>99</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>101</v>
       </c>
-      <c r="F5" t="s">
+      <c r="J5" t="s">
         <v>102</v>
-      </c>
-      <c r="G5" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" t="s">
-        <v>105</v>
-      </c>
-      <c r="J5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1713,13 +1713,13 @@
         <v>37</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1727,13 +1727,13 @@
         <v>40</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1741,13 +1741,13 @@
         <v>43</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1755,10 +1755,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1766,10 +1766,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1777,10 +1777,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1788,10 +1788,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1799,10 +1799,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1810,10 +1810,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1843,16 +1843,16 @@
         <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correctly identify farm device options and project variable names.
</commit_message>
<xml_diff>
--- a/dds/constants.xlsx
+++ b/dds/constants.xlsx
@@ -19,7 +19,7 @@
     <sheet name="Tables" sheetId="5" r:id="rId5"/>
     <sheet name="Valid Values" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="128">
   <si>
     <t>Identifier</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Table …</t>
   </si>
   <si>
-    <t>groutstr</t>
-  </si>
-  <si>
     <t>reynolds_number</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>Auto Only</t>
   </si>
   <si>
-    <t>reference.ref_general_parameter</t>
-  </si>
-  <si>
     <t>reference.ref_wake_amplification_factor_cyl</t>
   </si>
   <si>
@@ -416,6 +410,9 @@
   </si>
   <si>
     <t>reference.constants</t>
+  </si>
+  <si>
+    <t>grout_strength</t>
   </si>
 </sst>
 </file>
@@ -914,13 +911,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1595,7 +1592,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1633,10 +1630,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1644,19 +1641,19 @@
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" t="s">
         <v>88</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>89</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>90</v>
-      </c>
-      <c r="F3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1664,16 +1661,16 @@
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" t="s">
         <v>92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1681,31 +1678,31 @@
         <v>34</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" t="s">
         <v>95</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>96</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>97</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>98</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>99</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>100</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>101</v>
-      </c>
-      <c r="J5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1713,13 +1710,13 @@
         <v>37</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1727,13 +1724,13 @@
         <v>40</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" t="s">
         <v>103</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1741,13 +1738,13 @@
         <v>43</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
         <v>110</v>
-      </c>
-      <c r="D8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1755,10 +1752,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1766,10 +1763,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1777,10 +1774,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1788,10 +1785,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1799,10 +1796,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1810,10 +1807,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1843,16 +1840,16 @@
         <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>107</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Santise some variable fields.
</commit_message>
<xml_diff>
--- a/dds/constants.xlsx
+++ b/dds/constants.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="129">
   <si>
     <t>Identifier</t>
   </si>
@@ -274,12 +274,6 @@
     <t>Unit …</t>
   </si>
   <si>
-    <t>$m/s^{2}$</t>
-  </si>
-  <si>
-    <t>$kg/m^{3}$</t>
-  </si>
-  <si>
     <t>Table 1</t>
   </si>
   <si>
@@ -413,6 +407,15 @@
   </si>
   <si>
     <t>grout_strength</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>kg/m^{3}</t>
+  </si>
+  <si>
+    <t>m/s^{2}</t>
   </si>
 </sst>
 </file>
@@ -881,7 +884,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,13 +914,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1501,15 +1504,15 @@
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="1025" width="19.81640625"/>
   </cols>
   <sheetData>
@@ -1535,7 +1538,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1543,7 +1546,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1551,7 +1554,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1559,7 +1562,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1567,7 +1570,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1575,12 +1578,20 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1591,7 +1602,7 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1612,16 +1623,16 @@
         <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>86</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1630,10 +1641,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1641,19 +1652,19 @@
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" t="s">
         <v>87</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>88</v>
-      </c>
-      <c r="E3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F3" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -1661,16 +1672,16 @@
         <v>31</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
         <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1678,31 +1689,31 @@
         <v>34</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
         <v>94</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>95</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>96</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>97</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>98</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>99</v>
-      </c>
-      <c r="I5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J5" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1710,13 +1721,13 @@
         <v>37</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1724,13 +1735,13 @@
         <v>40</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1738,13 +1749,13 @@
         <v>43</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1752,10 +1763,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1763,10 +1774,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1774,10 +1785,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1785,10 +1796,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1796,10 +1807,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1807,10 +1818,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1840,16 +1851,16 @@
         <v>46</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove interpolation row from some of the moorings data and switch some of the structures to LineTables.
</commit_message>
<xml_diff>
--- a/dds/constants.xlsx
+++ b/dds/constants.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>constants.cylinder_drag</t>
   </si>
   <si>
-    <t>TableDataColumn</t>
-  </si>
-  <si>
     <t>Cylinder Drag Coefficients</t>
   </si>
   <si>
@@ -416,6 +413,9 @@
   </si>
   <si>
     <t>m/s^{2}</t>
+  </si>
+  <si>
+    <t>LineTableColumn</t>
   </si>
 </sst>
 </file>
@@ -882,9 +882,9 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -914,13 +914,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
@@ -1029,83 +1029,83 @@
         <v>27</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1133,19 +1133,19 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -1153,7 +1153,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1161,7 +1161,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1169,7 +1169,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1177,7 +1177,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1185,7 +1185,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1193,7 +1193,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1201,32 +1201,32 @@
         <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1234,42 +1234,42 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1280,13 +1280,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1318,7 +1318,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1352,31 +1352,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -1384,16 +1384,16 @@
         <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -1402,16 +1402,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1421,42 +1421,42 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1467,13 +1467,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1484,13 +1484,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +1506,7 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1518,19 +1518,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1538,7 +1538,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1546,7 +1546,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1554,7 +1554,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1562,7 +1562,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1570,7 +1570,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1578,7 +1578,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1586,7 +1586,7 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1620,19 +1620,19 @@
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1641,10 +1641,10 @@
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
         <v>124</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1652,110 +1652,110 @@
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
         <v>85</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>86</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>87</v>
-      </c>
-      <c r="F3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
         <v>89</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" t="s">
         <v>92</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>93</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>94</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>95</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>96</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>97</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>98</v>
-      </c>
-      <c r="J5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
         <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
         <v>107</v>
-      </c>
-      <c r="D8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1763,10 +1763,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1774,10 +1774,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1785,10 +1785,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1796,10 +1796,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1807,10 +1807,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1818,10 +1818,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1848,19 +1848,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix spelling of variable titles and descriptions and remove duplicate entry for bathymetry.layers
</commit_message>
<xml_diff>
--- a/dds/constants.xlsx
+++ b/dds/constants.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtopper\Programming\Python\git\dtocean-core\dds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\Python\git\dtocean-core\dds\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D789B4-B637-4669-A707-32AAA5DAAA2E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="409" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ROOT" sheetId="1" r:id="rId1"/>
@@ -124,12 +125,6 @@
     <t>constants.cylinder_wake_amplificiation</t>
   </si>
   <si>
-    <t>Cylinder Wake Amplificiation Factors</t>
-  </si>
-  <si>
-    <t>Cylinder wake amplificiation factors</t>
-  </si>
-  <si>
     <t>constants.rectangular_wind_drag</t>
   </si>
   <si>
@@ -416,19 +411,32 @@
   </si>
   <si>
     <t>LineTableColumn</t>
+  </si>
+  <si>
+    <t>Cylinder Wake Amplification Factors</t>
+  </si>
+  <si>
+    <t>Cylinder wake amplification factors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -504,15 +512,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -520,14 +528,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
@@ -876,7 +885,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -884,23 +893,23 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B14" sqref="B14"/>
+      <selection pane="topRight" activeCell="D10" sqref="C2:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="1021" width="19.81640625"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="1021" width="19.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -914,19 +923,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>5</v>
       </c>
@@ -940,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -954,7 +963,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -968,7 +977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
@@ -982,7 +991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>17</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>20</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>23</v>
       </c>
@@ -1024,12 +1033,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>28</v>
@@ -1038,74 +1047,74 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="10" t="s">
+    </row>
+    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="B11" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="10" t="s">
+    </row>
+    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="B12" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="B13" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="10" t="s">
+    </row>
+    <row r="14" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="B14" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1115,7 +1124,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1125,151 +1134,151 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.1796875"/>
-    <col min="2" max="1025" width="19.81640625"/>
+    <col min="1" max="1" width="38.140625"/>
+    <col min="2" max="1025" width="19.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1278,15 +1287,15 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1295,15 +1304,15 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1313,12 +1322,12 @@
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1328,7 +1337,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
@@ -1338,80 +1347,80 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1796875"/>
-    <col min="2" max="2" width="24.54296875"/>
-    <col min="3" max="3" width="34.1796875"/>
-    <col min="4" max="4" width="32.81640625"/>
-    <col min="5" max="5" width="26.81640625"/>
-    <col min="6" max="7" width="18.7265625"/>
-    <col min="8" max="9" width="19.7265625"/>
-    <col min="10" max="1025" width="8.453125"/>
+    <col min="1" max="1" width="36.140625"/>
+    <col min="2" max="2" width="24.5703125"/>
+    <col min="3" max="3" width="34.140625"/>
+    <col min="4" max="4" width="32.85546875"/>
+    <col min="5" max="5" width="26.85546875"/>
+    <col min="6" max="7" width="18.7109375"/>
+    <col min="8" max="9" width="19.7109375"/>
+    <col min="10" max="1025" width="8.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -1419,44 +1428,44 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1465,15 +1474,15 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1482,15 +1491,15 @@
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1500,7 +1509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1510,83 +1519,83 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="1025" width="19.81640625"/>
+    <col min="2" max="1025" width="19.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1606,222 +1615,222 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1796875"/>
-    <col min="2" max="2" width="43.54296875" customWidth="1"/>
-    <col min="3" max="3" width="25.453125"/>
-    <col min="4" max="4" width="39.26953125"/>
-    <col min="5" max="5" width="37.7265625"/>
-    <col min="6" max="8" width="21.453125"/>
-    <col min="9" max="10" width="22.453125"/>
-    <col min="11" max="1025" width="19.81640625"/>
+    <col min="1" max="1" width="36.140625"/>
+    <col min="2" max="2" width="43.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125"/>
+    <col min="4" max="4" width="39.28515625"/>
+    <col min="5" max="5" width="37.7109375"/>
+    <col min="6" max="8" width="21.42578125"/>
+    <col min="9" max="10" width="22.42578125"/>
+    <col min="11" max="1025" width="19.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>83</v>
-      </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>85</v>
       </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>89</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I5" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="C7" t="s">
         <v>97</v>
       </c>
-      <c r="J5" t="s">
+      <c r="D7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="9" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1831,7 +1840,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -1841,26 +1850,26 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="19.81640625"/>
+    <col min="1" max="1025" width="19.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>